<commit_message>
Change FOODON/Plant to PO/Whole plant (as plant is obsolete in FOODON)
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Product_Defs.xlsx
+++ b/inputs/AddictO_Product_Defs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharoncox/Documents/GitHub/addiction-ontology/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FCF9F9-6931-044D-85AB-A890BCEF9D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33591D10-F430-CE41-9A1F-EA1212679AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,12 @@
     <sheet name="Upper level diagram" sheetId="4" r:id="rId4"/>
     <sheet name="Links" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateCount="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="1023">
   <si>
     <t>ID</t>
   </si>
@@ -1968,21 +1968,9 @@
     <t>A product that is similar in appearance and physical substance to one used in an intervention but does not contain the active ingredient of that intervention.</t>
   </si>
   <si>
-    <t>FOODON_03411347</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
-    <t>A multicellular eukaryote organism of the kingdom Plantae.</t>
-  </si>
-  <si>
     <t>Organism</t>
   </si>
   <si>
-    <t xml:space="preserve">This needs to be revisited as FOODON is not necessarily the best source to import this entity from. </t>
-  </si>
-  <si>
     <t>SC/JH</t>
   </si>
   <si>
@@ -3097,6 +3085,15 @@
   </si>
   <si>
     <t>ChEBI definition does not highlight use for recretational purposes. Sold illcitly. Users seek out for its psychoactive properties. CHEBI: The principal psychoactive constituent of the cannabis plant, it is used for treatment of anorexia associated with AIDS as well as nausea and vomiting associated with cancer chemotherapy.</t>
+  </si>
+  <si>
+    <t>PO:0005679</t>
+  </si>
+  <si>
+    <t>Whole plant</t>
+  </si>
+  <si>
+    <t>A plant structure which is a whole organism.</t>
   </si>
 </sst>
 </file>
@@ -3734,10 +3731,10 @@
   <dimension ref="A1:X443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C231" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C302" sqref="C302"/>
+      <selection pane="bottomRight" activeCell="A237" sqref="A237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4100,13 +4097,13 @@
     <row r="10" spans="1:24" s="34" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="39"/>
       <c r="B10" s="34" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>51</v>
@@ -4115,10 +4112,10 @@
         <v>28</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
       <c r="S10" s="34" t="s">
         <v>40</v>
@@ -4136,7 +4133,7 @@
         <v>75</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="D11" s="41" t="s">
         <v>76</v>
@@ -4148,7 +4145,7 @@
         <v>28</v>
       </c>
       <c r="O11" s="41" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="S11" s="41" t="s">
         <v>40</v>
@@ -4426,10 +4423,10 @@
         <v>109</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>110</v>
@@ -4456,10 +4453,10 @@
     </row>
     <row r="23" spans="1:24" s="19" customFormat="1" ht="120" customHeight="1">
       <c r="B23" s="19" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>90</v>
@@ -4488,7 +4485,7 @@
         <v>116</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>90</v>
@@ -4517,7 +4514,7 @@
         <v>118</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>90</v>
@@ -4543,7 +4540,7 @@
         <v>120</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>90</v>
@@ -4555,7 +4552,7 @@
         <v>28</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="T26" s="19" t="s">
         <v>108</v>
@@ -4630,7 +4627,7 @@
         <v>125</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>126</v>
@@ -4645,7 +4642,7 @@
         <v>124</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="T30" s="19" t="s">
         <v>108</v>
@@ -4673,7 +4670,7 @@
         <v>129</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>130</v>
@@ -4785,13 +4782,13 @@
         <v>137</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="K36" s="19" t="s">
         <v>28</v>
@@ -4892,7 +4889,7 @@
         <v>147</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>148</v>
@@ -4910,7 +4907,7 @@
         <v>146</v>
       </c>
       <c r="O40" s="19" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="S40" s="19" t="s">
         <v>40</v>
@@ -6227,16 +6224,16 @@
     </row>
     <row r="92" spans="1:24" s="34" customFormat="1" ht="16">
       <c r="B92" s="34" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="D92" s="34" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="E92" s="34" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="K92" s="34" t="s">
         <v>28</v>
@@ -6303,22 +6300,22 @@
     </row>
     <row r="95" spans="1:24" s="8" customFormat="1" ht="53" customHeight="1">
       <c r="B95" s="8" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="C95" s="36" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="K95" s="8" t="s">
         <v>28</v>
       </c>
       <c r="O95" s="8" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="S95" s="8" t="s">
         <v>40</v>
@@ -6332,25 +6329,25 @@
     </row>
     <row r="96" spans="1:24" s="34" customFormat="1" ht="53" customHeight="1">
       <c r="B96" s="34" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
       <c r="C96" s="37" t="s">
+        <v>999</v>
+      </c>
+      <c r="D96" s="34" t="s">
         <v>1003</v>
       </c>
-      <c r="D96" s="34" t="s">
-        <v>1007</v>
-      </c>
       <c r="E96" s="34" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="K96" s="34" t="s">
         <v>28</v>
       </c>
       <c r="O96" s="38" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
       <c r="P96" s="34" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
       <c r="S96" s="34" t="s">
         <v>40</v>
@@ -6364,22 +6361,22 @@
     </row>
     <row r="97" spans="1:24" s="8" customFormat="1" ht="112">
       <c r="B97" s="8" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="C97" s="36" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="K97" s="8" t="s">
         <v>28</v>
       </c>
       <c r="O97" s="8" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="S97" s="8" t="s">
         <v>40</v>
@@ -8020,7 +8017,7 @@
         <v>466</v>
       </c>
       <c r="C157" s="19" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="D157" s="19" t="s">
         <v>467</v>
@@ -8038,7 +8035,7 @@
         <v>465</v>
       </c>
       <c r="O157" s="19" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="T157" s="19" t="s">
         <v>108</v>
@@ -8665,7 +8662,7 @@
         <v>534</v>
       </c>
       <c r="C186" s="19" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="D186" s="19" t="s">
         <v>535</v>
@@ -8680,7 +8677,7 @@
         <v>533</v>
       </c>
       <c r="O186" s="19" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="T186" s="19" t="s">
         <v>108</v>
@@ -8710,7 +8707,7 @@
         <v>538</v>
       </c>
       <c r="C188" s="19" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E188" s="19" t="s">
         <v>89</v>
@@ -8722,7 +8719,7 @@
         <v>537</v>
       </c>
       <c r="O188" s="19" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="T188" s="19" t="s">
         <v>108</v>
@@ -9842,35 +9839,29 @@
     </row>
     <row r="237" spans="1:24" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A237" s="19" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B237" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C237" s="19" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D237" s="19" t="s">
         <v>647</v>
-      </c>
-      <c r="B237" s="19" t="s">
-        <v>648</v>
-      </c>
-      <c r="C237" s="19" t="s">
-        <v>649</v>
-      </c>
-      <c r="D237" s="19" t="s">
-        <v>650</v>
       </c>
       <c r="E237" s="19" t="s">
         <v>89</v>
       </c>
       <c r="K237" s="19" t="s">
         <v>28</v>
-      </c>
-      <c r="L237" s="19" t="s">
-        <v>647</v>
-      </c>
-      <c r="M237" s="19" t="s">
-        <v>651</v>
       </c>
       <c r="O237" s="23"/>
       <c r="S237" s="19" t="s">
         <v>40</v>
       </c>
       <c r="T237" s="19" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="U237" s="19" t="s">
         <v>41</v>
@@ -9884,16 +9875,16 @@
     </row>
     <row r="239" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="A239" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B239" s="11" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C239" s="11" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D239" s="11" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="K239" s="11" t="s">
         <v>28</v>
@@ -9908,13 +9899,13 @@
     </row>
     <row r="240" spans="1:24" s="19" customFormat="1" ht="16">
       <c r="A240" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B240" s="19" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C240" s="19" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="D240" s="19" t="s">
         <v>208</v>
@@ -9926,7 +9917,7 @@
         <v>28</v>
       </c>
       <c r="N240" s="19" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="O240" s="23"/>
       <c r="S240" s="19">
@@ -9942,10 +9933,10 @@
     </row>
     <row r="241" spans="1:24" s="11" customFormat="1" ht="30" customHeight="1">
       <c r="B241" s="11" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="C241" s="11" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="K241" s="11" t="s">
         <v>28</v>
@@ -9961,7 +9952,7 @@
     </row>
     <row r="242" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B242" s="11" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="K242" s="11" t="s">
         <v>28</v>
@@ -9973,16 +9964,16 @@
     </row>
     <row r="243" spans="1:24" s="11" customFormat="1" ht="30" customHeight="1">
       <c r="A243" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B243" s="11" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="C243" s="11" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="D243" s="11" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="K243" s="11" t="s">
         <v>28</v>
@@ -9999,13 +9990,13 @@
     </row>
     <row r="244" spans="1:24" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A244" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B244" s="19" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C244" s="19" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D244" s="19" t="s">
         <v>558</v>
@@ -10017,7 +10008,7 @@
         <v>28</v>
       </c>
       <c r="N244" s="19" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="O244" s="23"/>
       <c r="S244" s="19" t="s">
@@ -10034,13 +10025,13 @@
     </row>
     <row r="245" spans="1:24" s="11" customFormat="1" ht="30" customHeight="1">
       <c r="B245" s="11" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C245" s="11" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="E245" s="11" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="K245" s="11" t="s">
         <v>28</v>
@@ -10059,13 +10050,13 @@
     </row>
     <row r="246" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="A246" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="B246" s="11" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C246" s="25" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D246" s="11" t="s">
         <v>281</v>
@@ -10088,13 +10079,13 @@
     </row>
     <row r="247" spans="1:24" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A247" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B247" s="19" t="s">
         <v>28</v>
       </c>
       <c r="C247" s="26" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="D247" s="19" t="s">
         <v>89</v>
@@ -10106,10 +10097,10 @@
         <v>28</v>
       </c>
       <c r="L247" s="27" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="M247" s="19" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="O247" s="23"/>
       <c r="S247" s="19" t="s">
@@ -10125,10 +10116,10 @@
     </row>
     <row r="248" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B248" s="11" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C248" s="25" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="K248" s="11" t="s">
         <v>28</v>
@@ -10143,10 +10134,10 @@
     </row>
     <row r="249" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B249" s="11" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C249" s="11" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="K249" s="11" t="s">
         <v>28</v>
@@ -10158,10 +10149,10 @@
     </row>
     <row r="250" spans="1:24" s="11" customFormat="1" ht="30" customHeight="1">
       <c r="B250" s="11" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C250" s="11" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="K250" s="11" t="s">
         <v>28</v>
@@ -10177,16 +10168,16 @@
     </row>
     <row r="251" spans="1:24" s="11" customFormat="1" ht="45" customHeight="1">
       <c r="A251" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B251" s="24" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="C251" s="24" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="D251" s="24" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="E251" s="24"/>
       <c r="F251" s="24"/>
@@ -10199,7 +10190,7 @@
       </c>
       <c r="L251" s="24"/>
       <c r="M251" s="24" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="N251" s="24"/>
       <c r="O251" s="24"/>
@@ -10213,7 +10204,7 @@
     </row>
     <row r="252" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B252" s="11" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="K252" s="11" t="s">
         <v>28</v>
@@ -10229,13 +10220,13 @@
     </row>
     <row r="253" spans="1:24" s="11" customFormat="1" ht="90" customHeight="1">
       <c r="A253" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B253" s="11" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="C253" s="11" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="D253" s="11" t="s">
         <v>193</v>
@@ -10247,10 +10238,10 @@
         <v>28</v>
       </c>
       <c r="L253" s="11" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="O253" s="11" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="U253" s="11" t="s">
         <v>41</v>
@@ -10259,7 +10250,7 @@
     </row>
     <row r="254" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B254" s="11" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="K254" s="11" t="s">
         <v>28</v>
@@ -10270,7 +10261,7 @@
     </row>
     <row r="255" spans="1:24" s="11" customFormat="1" ht="17" customHeight="1">
       <c r="B255" s="11" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="K255" s="11" t="s">
         <v>28</v>
@@ -10282,13 +10273,13 @@
     </row>
     <row r="256" spans="1:24" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A256" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B256" s="19" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="C256" s="19" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D256" s="19" t="s">
         <v>80</v>
@@ -10300,7 +10291,7 @@
         <v>28</v>
       </c>
       <c r="N256" s="19" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="O256" s="23"/>
       <c r="S256" s="19">
@@ -10315,13 +10306,13 @@
     </row>
     <row r="257" spans="1:24" s="19" customFormat="1" ht="16">
       <c r="A257" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B257" s="19" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="C257" s="19" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="D257" s="19" t="s">
         <v>206</v>
@@ -10333,7 +10324,7 @@
         <v>28</v>
       </c>
       <c r="N257" s="19" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="O257" s="23"/>
       <c r="S257" s="19">
@@ -10349,13 +10340,13 @@
     </row>
     <row r="258" spans="1:24" s="19" customFormat="1" ht="16">
       <c r="A258" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B258" s="19" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="C258" s="19" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D258" s="19" t="s">
         <v>208</v>
@@ -10367,7 +10358,7 @@
         <v>28</v>
       </c>
       <c r="N258" s="19" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="O258" s="23"/>
       <c r="S258" s="19">
@@ -10383,13 +10374,13 @@
     </row>
     <row r="259" spans="1:24" s="11" customFormat="1" ht="30" customHeight="1">
       <c r="A259" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B259" s="11" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="C259" s="11" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="D259" s="11" t="s">
         <v>208</v>
@@ -10411,7 +10402,7 @@
     </row>
     <row r="260" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B260" s="11" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="K260" s="11" t="s">
         <v>28</v>
@@ -10422,7 +10413,7 @@
     </row>
     <row r="261" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B261" s="11" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="K261" s="11" t="s">
         <v>28</v>
@@ -10438,7 +10429,7 @@
     </row>
     <row r="262" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B262" s="11" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="K262" s="11" t="s">
         <v>28</v>
@@ -10453,7 +10444,7 @@
     </row>
     <row r="263" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B263" s="11" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="K263" s="11" t="s">
         <v>28</v>
@@ -10465,7 +10456,7 @@
     </row>
     <row r="264" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B264" s="11" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="K264" s="11" t="s">
         <v>28</v>
@@ -10477,13 +10468,13 @@
     </row>
     <row r="265" spans="1:24" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A265" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B265" s="19" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="C265" s="19" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="D265" s="19" t="s">
         <v>256</v>
@@ -10495,10 +10486,10 @@
         <v>28</v>
       </c>
       <c r="N265" s="19" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="O265" s="19" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="S265" s="19" t="s">
         <v>40</v>
@@ -10513,7 +10504,7 @@
     </row>
     <row r="266" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B266" s="11" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="K266" s="11" t="s">
         <v>28</v>
@@ -10524,7 +10515,7 @@
     </row>
     <row r="267" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B267" s="11" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="K267" s="11" t="s">
         <v>28</v>
@@ -10539,7 +10530,7 @@
     </row>
     <row r="268" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B268" s="11" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="K268" s="11" t="s">
         <v>28</v>
@@ -10556,7 +10547,7 @@
     <row r="269" spans="1:24" s="8" customFormat="1" ht="16">
       <c r="A269" s="11"/>
       <c r="B269" s="11" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="C269" s="11"/>
       <c r="D269" s="11"/>
@@ -10589,7 +10580,7 @@
     </row>
     <row r="270" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B270" s="11" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="K270" s="11" t="s">
         <v>28</v>
@@ -10601,7 +10592,7 @@
     </row>
     <row r="271" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B271" s="11" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="K271" s="11" t="s">
         <v>28</v>
@@ -10613,13 +10604,13 @@
     </row>
     <row r="272" spans="1:24" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A272" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B272" s="19" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="C272" s="19" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D272" s="19" t="s">
         <v>208</v>
@@ -10631,7 +10622,7 @@
         <v>28</v>
       </c>
       <c r="N272" s="19" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="O272" s="23"/>
       <c r="S272" s="19">
@@ -10647,7 +10638,7 @@
     </row>
     <row r="273" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="B273" s="11" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="K273" s="11" t="s">
         <v>28</v>
@@ -10658,10 +10649,10 @@
     </row>
     <row r="274" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="A274" s="24" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="B274" s="11" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="K274" s="11" t="s">
         <v>28</v>
@@ -10673,13 +10664,13 @@
     </row>
     <row r="275" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A275" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="B275" s="19" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="C275" s="19" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D275" s="19" t="s">
         <v>208</v>
@@ -10704,7 +10695,7 @@
     </row>
     <row r="276" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="B276" s="11" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="K276" s="11" t="s">
         <v>28</v>
@@ -10715,13 +10706,13 @@
     </row>
     <row r="277" spans="1:23" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A277" s="23" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B277" s="19" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="C277" s="19" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D277" s="19" t="s">
         <v>384</v>
@@ -10733,7 +10724,7 @@
         <v>28</v>
       </c>
       <c r="O277" s="23" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="S277" s="19">
         <v>1</v>
@@ -10748,7 +10739,7 @@
     </row>
     <row r="278" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="B278" s="11" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="K278" s="11" t="s">
         <v>28</v>
@@ -10759,28 +10750,28 @@
     </row>
     <row r="279" spans="1:23" s="11" customFormat="1" ht="33" customHeight="1">
       <c r="A279" t="s">
+        <v>742</v>
+      </c>
+      <c r="B279" s="11" t="s">
+        <v>743</v>
+      </c>
+      <c r="C279" s="11" t="s">
+        <v>744</v>
+      </c>
+      <c r="D279" s="11" t="s">
+        <v>745</v>
+      </c>
+      <c r="E279" s="11" t="s">
         <v>746</v>
       </c>
-      <c r="B279" s="11" t="s">
+      <c r="K279" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L279" s="11" t="s">
         <v>747</v>
       </c>
-      <c r="C279" s="11" t="s">
+      <c r="N279" s="11" t="s">
         <v>748</v>
-      </c>
-      <c r="D279" s="11" t="s">
-        <v>749</v>
-      </c>
-      <c r="E279" s="11" t="s">
-        <v>750</v>
-      </c>
-      <c r="K279" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L279" s="11" t="s">
-        <v>751</v>
-      </c>
-      <c r="N279" s="11" t="s">
-        <v>752</v>
       </c>
       <c r="U279" s="11" t="s">
         <v>41</v>
@@ -10788,16 +10779,16 @@
     </row>
     <row r="280" spans="1:23" s="19" customFormat="1" ht="33" customHeight="1">
       <c r="A280" s="19" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="B280" s="19" t="s">
         <v>225</v>
       </c>
       <c r="C280" s="19" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D280" s="19" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="E280" s="19" t="s">
         <v>27</v>
@@ -10809,7 +10800,7 @@
         <v>28</v>
       </c>
       <c r="L280" s="19" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="S280" s="19" t="s">
         <v>40</v>
@@ -10823,13 +10814,13 @@
     </row>
     <row r="281" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A281" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B281" s="19" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="C281" s="19" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="D281" s="19" t="s">
         <v>256</v>
@@ -10841,7 +10832,7 @@
         <v>28</v>
       </c>
       <c r="N281" s="19" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="O281" s="23"/>
       <c r="S281" s="19">
@@ -10856,13 +10847,13 @@
     </row>
     <row r="282" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A282" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="B282" s="19" t="s">
         <v>204</v>
       </c>
       <c r="C282" s="19" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="D282" s="19" t="s">
         <v>256</v>
@@ -10887,13 +10878,13 @@
     </row>
     <row r="283" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A283" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="B283" s="19" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="C283" s="19" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="D283" s="19" t="s">
         <v>28</v>
@@ -10918,13 +10909,13 @@
     </row>
     <row r="284" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A284" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B284" s="19" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="C284" s="19" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="D284" s="19" t="s">
         <v>204</v>
@@ -10949,13 +10940,13 @@
     </row>
     <row r="285" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A285" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="B285" s="19" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="C285" s="19" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="D285" s="19" t="s">
         <v>204</v>
@@ -10980,13 +10971,13 @@
     </row>
     <row r="286" spans="1:23" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A286" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="B286" s="19" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="C286" s="19" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="D286" s="19" t="s">
         <v>80</v>
@@ -11010,7 +11001,7 @@
     </row>
     <row r="287" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="B287" s="11" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="K287" s="11" t="s">
         <v>28</v>
@@ -11023,7 +11014,7 @@
     <row r="288" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="A288" s="24"/>
       <c r="B288" s="11" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="K288" s="11" t="s">
         <v>28</v>
@@ -11034,7 +11025,7 @@
     </row>
     <row r="289" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B289" s="11" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="K289" s="11" t="s">
         <v>28</v>
@@ -11046,7 +11037,7 @@
     <row r="290" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="A290" s="8"/>
       <c r="B290" s="11" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="K290" s="11" t="s">
         <v>28</v>
@@ -11059,7 +11050,7 @@
     </row>
     <row r="291" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B291" s="11" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="K291" s="11" t="s">
         <v>28</v>
@@ -11070,13 +11061,13 @@
     </row>
     <row r="292" spans="1:24" s="19" customFormat="1" ht="60" customHeight="1">
       <c r="A292" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="B292" s="19" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="C292" s="19" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="D292" s="19" t="s">
         <v>477</v>
@@ -11088,7 +11079,7 @@
         <v>28</v>
       </c>
       <c r="O292" s="19" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="T292" s="19" t="s">
         <v>108</v>
@@ -11100,7 +11091,7 @@
     </row>
     <row r="293" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B293" s="11" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="K293" s="11" t="s">
         <v>28</v>
@@ -11111,13 +11102,13 @@
     </row>
     <row r="294" spans="1:24" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A294" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B294" s="19" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="C294" s="19" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="D294" s="19" t="s">
         <v>76</v>
@@ -11129,18 +11120,18 @@
         <v>28</v>
       </c>
       <c r="N294" s="19" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
     </row>
     <row r="295" spans="1:24" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A295" s="19" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B295" s="23" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C295" s="23" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D295" s="23" t="s">
         <v>158</v>
@@ -11157,7 +11148,7 @@
         <v>28</v>
       </c>
       <c r="L295" s="23" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="M295" s="23"/>
       <c r="N295" s="23"/>
@@ -11176,7 +11167,7 @@
     </row>
     <row r="296" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B296" s="11" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="K296" s="11" t="s">
         <v>28</v>
@@ -11188,7 +11179,7 @@
     </row>
     <row r="297" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B297" s="24" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="C297" s="24"/>
       <c r="D297" s="24"/>
@@ -11215,7 +11206,7 @@
     </row>
     <row r="298" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B298" s="11" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="K298" s="11" t="s">
         <v>28</v>
@@ -11227,7 +11218,7 @@
     </row>
     <row r="299" spans="1:24" s="11" customFormat="1" ht="16">
       <c r="B299" s="11" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="D299" s="11" t="s">
         <v>58</v>
@@ -11242,13 +11233,13 @@
     </row>
     <row r="300" spans="1:24" s="19" customFormat="1" ht="16">
       <c r="A300" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="B300" s="19" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="C300" s="19" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D300" s="19" t="s">
         <v>208</v>
@@ -11272,13 +11263,13 @@
     </row>
     <row r="301" spans="1:24" s="19" customFormat="1" ht="90" customHeight="1">
       <c r="A301" s="19" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B301" s="19" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C301" s="19" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="D301" s="19" t="s">
         <v>158</v>
@@ -11290,13 +11281,13 @@
         <v>28</v>
       </c>
       <c r="L301" s="19" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="N301" s="19" t="s">
         <v>161</v>
       </c>
       <c r="O301" s="23" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="S301" s="19" t="s">
         <v>40</v>
@@ -11312,16 +11303,16 @@
     </row>
     <row r="302" spans="1:24" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A302" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B302" s="19" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="C302" s="19" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D302" s="19" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="E302" s="19" t="s">
         <v>89</v>
@@ -11342,13 +11333,13 @@
     </row>
     <row r="303" spans="1:24" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A303" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B303" s="19" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="C303" s="26" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="D303" s="19" t="s">
         <v>287</v>
@@ -11376,16 +11367,16 @@
     </row>
     <row r="304" spans="1:24" s="19" customFormat="1" ht="16">
       <c r="A304" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B304" s="19" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="C304" s="26" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="D304" s="19" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="E304" s="19" t="s">
         <v>89</v>
@@ -11409,13 +11400,13 @@
     </row>
     <row r="305" spans="1:23" s="19" customFormat="1" ht="16">
       <c r="A305" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B305" s="19" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="C305" s="19" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="D305" s="19" t="s">
         <v>28</v>
@@ -11424,7 +11415,7 @@
         <v>89</v>
       </c>
       <c r="G305" s="19" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="K305" s="19" t="s">
         <v>28</v>
@@ -11448,13 +11439,13 @@
     </row>
     <row r="307" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A307" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B307" s="19" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="C307" s="19" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="D307" s="19" t="s">
         <v>28</v>
@@ -11463,7 +11454,7 @@
         <v>89</v>
       </c>
       <c r="G307" s="19" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="K307" s="19" t="s">
         <v>28</v>
@@ -11481,16 +11472,16 @@
     </row>
     <row r="308" spans="1:23" s="19" customFormat="1" ht="135" customHeight="1">
       <c r="A308" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="B308" s="19" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="C308" s="19" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="D308" s="19" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="E308" s="19" t="s">
         <v>89</v>
@@ -11499,10 +11490,10 @@
         <v>28</v>
       </c>
       <c r="N308" s="19" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="O308" s="23" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="S308" s="19" t="s">
         <v>40</v>
@@ -11516,16 +11507,16 @@
     </row>
     <row r="309" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A309" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B309" s="19" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C309" s="26" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D309" s="19" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="E309" s="19" t="s">
         <v>27</v>
@@ -11546,13 +11537,13 @@
     </row>
     <row r="310" spans="1:23" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A310" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B310" s="19" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="C310" s="26" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D310" s="19" t="s">
         <v>28</v>
@@ -11561,13 +11552,13 @@
         <v>27</v>
       </c>
       <c r="H310" s="19" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="K310" s="19" t="s">
         <v>28</v>
       </c>
       <c r="O310" s="23" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="T310" s="19" t="s">
         <v>108</v>
@@ -11575,13 +11566,13 @@
     </row>
     <row r="311" spans="1:23" s="19" customFormat="1" ht="75" customHeight="1">
       <c r="A311" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B311" s="19" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="C311" s="26" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D311" s="19" t="s">
         <v>28</v>
@@ -11593,7 +11584,7 @@
         <v>28</v>
       </c>
       <c r="O311" s="23" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="S311" s="19" t="s">
         <v>40</v>
@@ -11607,16 +11598,16 @@
     </row>
     <row r="312" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A312" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B312" s="19" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="C312" s="19" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D312" s="19" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="E312" s="19" t="s">
         <v>27</v>
@@ -11638,19 +11629,19 @@
     </row>
     <row r="313" spans="1:23" s="19" customFormat="1" ht="16">
       <c r="A313" t="s">
+        <v>834</v>
+      </c>
+      <c r="B313" s="19" t="s">
+        <v>835</v>
+      </c>
+      <c r="C313" s="19" t="s">
+        <v>836</v>
+      </c>
+      <c r="D313" s="19" t="s">
+        <v>837</v>
+      </c>
+      <c r="E313" s="19" t="s">
         <v>838</v>
-      </c>
-      <c r="B313" s="19" t="s">
-        <v>839</v>
-      </c>
-      <c r="C313" s="19" t="s">
-        <v>840</v>
-      </c>
-      <c r="D313" s="19" t="s">
-        <v>841</v>
-      </c>
-      <c r="E313" s="19" t="s">
-        <v>842</v>
       </c>
       <c r="K313" s="19" t="s">
         <v>28</v>
@@ -11668,13 +11659,13 @@
     </row>
     <row r="314" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A314" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B314" s="19" t="s">
         <v>456</v>
       </c>
       <c r="C314" s="19" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="D314" s="19" t="s">
         <v>28</v>
@@ -11683,13 +11674,13 @@
         <v>27</v>
       </c>
       <c r="H314" s="19" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="K314" s="19" t="s">
         <v>28</v>
       </c>
       <c r="N314" s="19" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="O314" s="23"/>
       <c r="S314" s="19">
@@ -11704,16 +11695,16 @@
     </row>
     <row r="315" spans="1:23" s="19" customFormat="1" ht="16">
       <c r="A315" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="B315" s="19" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="C315" s="19" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="D315" s="19" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="E315" s="19" t="s">
         <v>89</v>
@@ -11734,13 +11725,13 @@
     </row>
     <row r="316" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A316" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B316" s="19" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="C316" s="19" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="D316" s="19" t="s">
         <v>587</v>
@@ -11755,7 +11746,7 @@
         <v>28</v>
       </c>
       <c r="N316" s="19" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="O316" s="23"/>
       <c r="S316" s="19">
@@ -11771,13 +11762,13 @@
     </row>
     <row r="317" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A317" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B317" s="19" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="C317" s="19" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="D317" s="19" t="s">
         <v>225</v>
@@ -11786,7 +11777,7 @@
         <v>27</v>
       </c>
       <c r="H317" s="19" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="O317" s="23"/>
       <c r="S317" s="19" t="s">
@@ -11802,7 +11793,7 @@
     </row>
     <row r="318" spans="1:23" s="13" customFormat="1" ht="16">
       <c r="B318" s="13" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="K318" s="13" t="s">
         <v>28</v>
@@ -11817,7 +11808,7 @@
     </row>
     <row r="319" spans="1:23" s="11" customFormat="1" ht="16">
       <c r="B319" s="11" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="K319" s="11" t="s">
         <v>28</v>
@@ -11833,13 +11824,13 @@
     </row>
     <row r="320" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A320" s="19" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="B320" s="19" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="C320" s="19" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="D320" s="19" t="s">
         <v>110</v>
@@ -11867,13 +11858,13 @@
     </row>
     <row r="321" spans="1:23" s="19" customFormat="1" ht="16">
       <c r="A321" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="B321" s="19" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="C321" s="19" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="D321" s="19" t="s">
         <v>208</v>
@@ -11885,7 +11876,7 @@
         <v>28</v>
       </c>
       <c r="N321" s="19" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="O321" s="23"/>
       <c r="S321" s="19">
@@ -11901,22 +11892,22 @@
     </row>
     <row r="322" spans="1:23" s="19" customFormat="1" ht="30" customHeight="1">
       <c r="A322" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
       <c r="B322" s="19" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="C322" s="19" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="D322" s="19" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="E322" s="19" t="s">
         <v>89</v>
       </c>
       <c r="H322" s="19" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="K322" s="19" t="s">
         <v>28</v>
@@ -11935,16 +11926,16 @@
     </row>
     <row r="323" spans="1:23" s="19" customFormat="1" ht="16">
       <c r="A323" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="B323" s="19" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="C323" s="19" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="D323" s="19" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="E323" s="19" t="s">
         <v>89</v>
@@ -11966,16 +11957,16 @@
     </row>
     <row r="324" spans="1:23" s="19" customFormat="1" ht="45" customHeight="1">
       <c r="A324" s="19" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B324" s="19" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="C324" s="19" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="D324" s="19" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="E324" s="19" t="s">
         <v>89</v>
@@ -11984,10 +11975,10 @@
         <v>28</v>
       </c>
       <c r="L324" s="19" t="s">
+        <v>870</v>
+      </c>
+      <c r="M324" s="19" t="s">
         <v>874</v>
-      </c>
-      <c r="M324" s="19" t="s">
-        <v>878</v>
       </c>
       <c r="O324" s="23"/>
       <c r="S324" s="19" t="s">
@@ -14557,16 +14548,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" ht="16">
       <c r="A1" s="4" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" customHeight="1">
@@ -14574,10 +14565,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1">
@@ -14585,10 +14576,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" customHeight="1">
@@ -14596,13 +14587,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1">
@@ -14610,10 +14601,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" customHeight="1">
@@ -14621,13 +14612,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1">
@@ -14635,10 +14626,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" customHeight="1">
@@ -14646,10 +14637,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16">
@@ -14657,10 +14648,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1">
@@ -14668,10 +14659,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1">
@@ -14679,10 +14670,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16">
@@ -14690,10 +14681,10 @@
         <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1">
@@ -14701,10 +14692,10 @@
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" customHeight="1">
@@ -14712,10 +14703,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1">
@@ -14723,10 +14714,10 @@
         <v>18</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16">
@@ -14734,10 +14725,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1">
@@ -14745,10 +14736,10 @@
         <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16">
@@ -14756,10 +14747,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1">
@@ -14767,10 +14758,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
     </row>
   </sheetData>
@@ -14814,16 +14805,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>12</v>
@@ -14838,18 +14829,18 @@
         <v>15</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
@@ -14857,13 +14848,13 @@
     </row>
     <row r="3" spans="1:12" ht="60" customHeight="1">
       <c r="B3" s="1" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -14871,16 +14862,16 @@
     </row>
     <row r="4" spans="1:12" ht="45" customHeight="1">
       <c r="B4" s="1" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -14888,30 +14879,30 @@
     </row>
     <row r="5" spans="1:12" ht="16">
       <c r="B5" s="1" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="16">
       <c r="B6" s="1" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="16">
       <c r="B7" s="1" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="16">
       <c r="B8" s="1" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60" customHeight="1">
       <c r="B9" s="1" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
@@ -14919,13 +14910,13 @@
     </row>
     <row r="10" spans="1:12" ht="45" customHeight="1">
       <c r="B10" s="1" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="L10" s="1">
         <v>1</v>
@@ -14933,16 +14924,16 @@
     </row>
     <row r="11" spans="1:12" ht="45" customHeight="1">
       <c r="B11" s="1" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="L11" s="1">
         <v>1</v>
@@ -14950,13 +14941,13 @@
     </row>
     <row r="12" spans="1:12" ht="16">
       <c r="B12" s="1" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="L12" s="1">
         <v>1</v>
@@ -14964,13 +14955,13 @@
     </row>
     <row r="13" spans="1:12" ht="45" customHeight="1">
       <c r="B13" s="1" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -14981,13 +14972,13 @@
     </row>
     <row r="14" spans="1:12" ht="51" customHeight="1">
       <c r="B14" s="1" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -15028,37 +15019,37 @@
   <sheetData>
     <row r="1" spans="1:11" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>948</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>949</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>950</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>951</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>952</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>953</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>954</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>955</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>956</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>957</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>958</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>959</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -15066,7 +15057,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
@@ -15077,16 +15068,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C3" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -15094,16 +15085,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C4" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -15111,16 +15102,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>959</v>
+      </c>
+      <c r="C5" t="s">
+        <v>960</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
         <v>963</v>
-      </c>
-      <c r="C5" t="s">
-        <v>964</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -15128,16 +15119,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C6" t="s">
+        <v>960</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
         <v>964</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -15145,16 +15136,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C7" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -15162,10 +15153,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C8" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -15179,16 +15170,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C9" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -15196,16 +15187,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C10" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -15213,16 +15204,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="C11" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -15230,7 +15221,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -15242,13 +15233,13 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="J12" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="K12" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -15256,7 +15247,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -15268,13 +15259,13 @@
         <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J13" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K13" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -15282,7 +15273,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -15294,13 +15285,13 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J14" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K14" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -15308,7 +15299,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -15320,13 +15311,13 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J15" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K15" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -15334,7 +15325,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -15346,13 +15337,13 @@
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J16" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K16" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -15360,7 +15351,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -15372,13 +15363,13 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J17" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K17" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -15386,7 +15377,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -15398,13 +15389,13 @@
         <v>6</v>
       </c>
       <c r="I18" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J18" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K18" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -15412,7 +15403,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -15424,13 +15415,13 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J19" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K19" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -15438,7 +15429,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -15450,13 +15441,13 @@
         <v>9</v>
       </c>
       <c r="I20" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J20" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K20" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -15464,7 +15455,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -15476,13 +15467,13 @@
         <v>7</v>
       </c>
       <c r="I21" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="J21" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="K21" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -15490,7 +15481,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -15502,13 +15493,13 @@
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="J22" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="K22" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -15516,7 +15507,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -15528,13 +15519,13 @@
         <v>7</v>
       </c>
       <c r="I23" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J23" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K23" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -15542,7 +15533,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -15554,13 +15545,13 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J24" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K24" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -15568,7 +15559,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -15580,13 +15571,13 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J25" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K25" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -15594,7 +15585,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -15606,13 +15597,13 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J26" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K26" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -15620,7 +15611,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -15632,13 +15623,13 @@
         <v>7</v>
       </c>
       <c r="I27" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J27" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K27" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -15646,7 +15637,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -15658,13 +15649,13 @@
         <v>9</v>
       </c>
       <c r="I28" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J28" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K28" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -15672,7 +15663,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -15684,13 +15675,13 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J29" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K29" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -15698,7 +15689,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -15710,13 +15701,13 @@
         <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="J30" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="K30" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>